<commit_message>
Added Diagrams to Hardward in PDR, still need bluetooth diagram
</commit_message>
<xml_diff>
--- a/Connections_Table.xlsx
+++ b/Connections_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11600"/>
   </bookViews>
   <sheets>
     <sheet name="p1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="89">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t xml:space="preserve">LCD (2), Phototransistor1,2,3 [C], IR LED1,2,3(+) </t>
+  </si>
+  <si>
+    <t>Phototransistor3(front)</t>
+  </si>
+  <si>
+    <t>Phototransistor2(right)</t>
+  </si>
+  <si>
+    <t>Phototransistor1(left)</t>
   </si>
 </sst>
 </file>
@@ -654,31 +663,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -730,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4</v>
       </c>
@@ -763,7 +772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -803,7 +812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:A24" si="0">A4+2</f>
         <v>8</v>
@@ -843,7 +852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -883,7 +892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -923,7 +932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -963,7 +972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1003,7 +1012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1043,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1083,7 +1092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1123,7 +1132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1163,7 +1172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1203,7 +1212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1243,7 +1252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1283,7 +1292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1323,7 +1332,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1363,7 +1372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1385,7 +1394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1408,7 +1417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1430,7 +1439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1451,7 +1460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1473,7 +1482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1495,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <f>A24+2</f>
         <v>48</v>
@@ -1517,7 +1526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1529,7 +1538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1541,7 +1550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1553,7 +1562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>49</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>52</v>
       </c>
@@ -1621,13 +1630,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
         <v>65</v>
@@ -1639,7 +1648,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1677,7 +1686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -1753,9 +1762,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
         <v>66</v>
@@ -1767,7 +1776,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1843,7 +1852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1881,9 +1890,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E48" t="s">
         <v>67</v>
@@ -1895,7 +1904,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1971,7 +1980,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -2022,12 +2031,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2041,7 +2050,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2079,7 +2088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2117,7 +2126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2204,7 +2213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -2242,7 +2251,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -2277,7 +2286,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2291,7 +2300,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Hardware portion for PDR complete
</commit_message>
<xml_diff>
--- a/Connections_Table.xlsx
+++ b/Connections_Table.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="p1" sheetId="1" r:id="rId1"/>
     <sheet name="Transistors_LED" sheetId="3" r:id="rId2"/>
+    <sheet name="p2_BT" sheetId="4" r:id="rId3"/>
+    <sheet name="Parts" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="101">
   <si>
     <t>Expansion Board J11</t>
   </si>
@@ -292,12 +294,51 @@
   </si>
   <si>
     <t>Phototransistor1(left)</t>
+  </si>
+  <si>
+    <t>BT (MOSI)</t>
+  </si>
+  <si>
+    <t>BT (MISO)</t>
+  </si>
+  <si>
+    <t>BT (SCK)</t>
+  </si>
+  <si>
+    <t>BT(CS)</t>
+  </si>
+  <si>
+    <t>Parts List</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Approx. Cost</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Adafruit Bluefruit LE SPI Friend - Bluetooth Low Energy (BLE)</t>
+  </si>
+  <si>
+    <t>adafruit.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -381,6 +422,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,31 +705,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection sqref="A1:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -739,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -772,7 +814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>6</v>
@@ -812,7 +854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A24" si="0">A4+2</f>
         <v>8</v>
@@ -852,7 +894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -892,7 +934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -932,7 +974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -972,7 +1014,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1012,7 +1054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1052,7 +1094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1092,7 +1134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1132,7 +1174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1172,7 +1214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1212,7 +1254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1252,7 +1294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1292,7 +1334,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1332,7 +1374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1372,7 +1414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1394,7 +1436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1417,7 +1459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1439,7 +1481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1460,7 +1502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1482,7 +1524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1504,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>A24+2</f>
         <v>48</v>
@@ -1526,7 +1568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -1538,7 +1580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E27">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -1550,7 +1592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E28">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -1562,7 +1604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1570,7 +1612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1590,7 +1632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>49</v>
       </c>
@@ -1610,7 +1652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>52</v>
       </c>
@@ -1630,11 +1672,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -1648,7 +1690,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1686,7 +1728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -1724,7 +1766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -1762,7 +1804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -1776,7 +1818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1814,7 +1856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1852,7 +1894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1890,7 +1932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -1904,7 +1946,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1942,7 +1984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1980,7 +2022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -2028,15 +2070,15 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2050,7 +2092,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2088,7 +2130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2126,7 +2168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2161,7 +2203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -2175,7 +2217,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2213,7 +2255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -2251,7 +2293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -2286,7 +2328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2300,7 +2342,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2338,7 +2380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2376,7 +2418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -2409,6 +2451,650 @@
       </c>
       <c r="O16" s="6" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+2</f>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <f>E3+2</f>
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A24" si="0">A4+2</f>
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E21" si="1">E4+2</f>
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <f>E22+2</f>
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E28" si="2">E23+2</f>
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>A24+2</f>
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>2633</v>
+      </c>
+      <c r="D3" s="10">
+        <v>17.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>